<commit_message>
Remove back to front sorting.
</commit_message>
<xml_diff>
--- a/P3DFps.xlsx
+++ b/P3DFps.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zak\Documents\GitProjects\Potato3d\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{130E1E26-2203-4DD0-A2BD-834169B07FC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC4439A2-6D82-4568-B839-DFB9A0C85AD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2904C00D-6B2E-49C9-A39A-1A4D989C3045}"/>
+    <workbookView xWindow="1305" yWindow="1515" windowWidth="21570" windowHeight="11370" xr2:uid="{2904C00D-6B2E-49C9-A39A-1A4D989C3045}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
   <si>
     <t>BSP</t>
   </si>
@@ -95,6 +95,12 @@
   </si>
   <si>
     <t>s_opening</t>
+  </si>
+  <si>
+    <t>oFast</t>
+  </si>
+  <si>
+    <t>Combine uv mask</t>
   </si>
 </sst>
 </file>
@@ -4213,10 +4219,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A9F04DC-EF96-45BA-9879-6DBCF76CA793}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4242,7 +4248,7 @@
         <v>305</v>
       </c>
       <c r="C2" s="1">
-        <f t="shared" ref="C2:C19" si="0">B2/30</f>
+        <f t="shared" ref="C2:C22" si="0">B2/30</f>
         <v>10.166666666666666</v>
       </c>
       <c r="D2" s="2">
@@ -4355,7 +4361,7 @@
         <v>10.966666666666667</v>
       </c>
       <c r="D9" s="2">
-        <f t="shared" ref="D9:D19" si="2">B9/$B$2</f>
+        <f t="shared" ref="D9:D22" si="2">B9/$B$2</f>
         <v>1.0786885245901638</v>
       </c>
     </row>
@@ -4517,6 +4523,54 @@
       <c r="D19" s="2">
         <f t="shared" si="2"/>
         <v>0.88524590163934425</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20">
+        <v>278</v>
+      </c>
+      <c r="C20" s="1">
+        <f t="shared" si="0"/>
+        <v>9.2666666666666675</v>
+      </c>
+      <c r="D20" s="2">
+        <f t="shared" si="2"/>
+        <v>0.91147540983606556</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21">
+        <v>279</v>
+      </c>
+      <c r="C21" s="1">
+        <f t="shared" si="0"/>
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="D21" s="2">
+        <f t="shared" si="2"/>
+        <v>0.91475409836065569</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22">
+        <v>280</v>
+      </c>
+      <c r="C22" s="1">
+        <f t="shared" si="0"/>
+        <v>9.3333333333333339</v>
+      </c>
+      <c r="D22" s="2">
+        <f t="shared" si="2"/>
+        <v>0.91803278688524592</v>
       </c>
     </row>
   </sheetData>
@@ -4942,7 +4996,7 @@
         <v>719</v>
       </c>
       <c r="D37">
-        <f t="shared" ref="D37:D39" si="5">C37-B37+1</f>
+        <f t="shared" ref="D37:D38" si="5">C37-B37+1</f>
         <v>702</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Only use perspective correct every 8px.
</commit_message>
<xml_diff>
--- a/P3DFps.xlsx
+++ b/P3DFps.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zak\Documents\GitProjects\Potato3d\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC4439A2-6D82-4568-B839-DFB9A0C85AD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84B5D465-8CEE-438D-8EFC-C78D3D182453}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1305" yWindow="1515" windowWidth="21570" windowHeight="11370" xr2:uid="{2904C00D-6B2E-49C9-A39A-1A4D989C3045}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2904C00D-6B2E-49C9-A39A-1A4D989C3045}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
   <si>
     <t>BSP</t>
   </si>
@@ -101,6 +101,9 @@
   </si>
   <si>
     <t>Combine uv mask</t>
+  </si>
+  <si>
+    <t>Perspective Correct</t>
   </si>
 </sst>
 </file>
@@ -4219,10 +4222,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A9F04DC-EF96-45BA-9879-6DBCF76CA793}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4248,7 +4251,7 @@
         <v>305</v>
       </c>
       <c r="C2" s="1">
-        <f t="shared" ref="C2:C22" si="0">B2/30</f>
+        <f t="shared" ref="C2:C23" si="0">B2/30</f>
         <v>10.166666666666666</v>
       </c>
       <c r="D2" s="2">
@@ -4361,7 +4364,7 @@
         <v>10.966666666666667</v>
       </c>
       <c r="D9" s="2">
-        <f t="shared" ref="D9:D22" si="2">B9/$B$2</f>
+        <f t="shared" ref="D9:D23" si="2">B9/$B$2</f>
         <v>1.0786885245901638</v>
       </c>
     </row>
@@ -4571,6 +4574,22 @@
       <c r="D22" s="2">
         <f t="shared" si="2"/>
         <v>0.91803278688524592</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23">
+        <v>181</v>
+      </c>
+      <c r="C23" s="1">
+        <f t="shared" si="0"/>
+        <v>6.0333333333333332</v>
+      </c>
+      <c r="D23" s="2">
+        <f t="shared" si="2"/>
+        <v>0.59344262295081962</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Only perspective correct every 16px.
</commit_message>
<xml_diff>
--- a/P3DFps.xlsx
+++ b/P3DFps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zak\Documents\GitProjects\Potato3d\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11986F4C-5D95-44B7-9396-4228CC0C6DE2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD45FE8-E90D-413B-932F-4EEE9EBFE6B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2904C00D-6B2E-49C9-A39A-1A4D989C3045}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
   <si>
     <t>BSP</t>
   </si>
@@ -107,6 +107,9 @@
   </si>
   <si>
     <t>Reciprocal table</t>
+  </si>
+  <si>
+    <t>16x perspective</t>
   </si>
 </sst>
 </file>
@@ -4225,10 +4228,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A9F04DC-EF96-45BA-9879-6DBCF76CA793}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4254,7 +4257,7 @@
         <v>305</v>
       </c>
       <c r="C2" s="1">
-        <f t="shared" ref="C2:C25" si="0">B2/30</f>
+        <f t="shared" ref="C2:C26" si="0">B2/30</f>
         <v>10.166666666666666</v>
       </c>
       <c r="D2" s="2">
@@ -4367,7 +4370,7 @@
         <v>10.966666666666667</v>
       </c>
       <c r="D9" s="2">
-        <f t="shared" ref="D9:D25" si="2">B9/$B$2</f>
+        <f t="shared" ref="D9:D26" si="2">B9/$B$2</f>
         <v>1.0786885245901638</v>
       </c>
     </row>
@@ -4625,6 +4628,22 @@
       <c r="D25" s="2">
         <f t="shared" si="2"/>
         <v>0.75737704918032789</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>243</v>
+      </c>
+      <c r="C26" s="1">
+        <f t="shared" si="0"/>
+        <v>8.1</v>
+      </c>
+      <c r="D26" s="2">
+        <f t="shared" si="2"/>
+        <v>0.79672131147540981</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove perspective correct flags
</commit_message>
<xml_diff>
--- a/P3DFps.xlsx
+++ b/P3DFps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zak\Documents\GitProjects\Potato3d\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD45FE8-E90D-413B-932F-4EEE9EBFE6B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2DF3676-B27B-4470-905B-F659B47C7CEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2904C00D-6B2E-49C9-A39A-1A4D989C3045}"/>
   </bookViews>
@@ -4231,7 +4231,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
More efficient vector delete.
</commit_message>
<xml_diff>
--- a/P3DFps.xlsx
+++ b/P3DFps.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zak\Documents\GitProjects\Potato3d\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ABC72D1-E5A1-460A-94DD-8C8BDE793501}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE09B382-6460-4F2D-80D0-D50841C0D5A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10515" yWindow="480" windowWidth="21570" windowHeight="11370" xr2:uid="{2904C00D-6B2E-49C9-A39A-1A4D989C3045}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2904C00D-6B2E-49C9-A39A-1A4D989C3045}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>BSP</t>
   </si>
@@ -106,6 +106,12 @@
   </si>
   <si>
     <t>Consolidate spans</t>
+  </si>
+  <si>
+    <t>Consolidate spans2</t>
+  </si>
+  <si>
+    <t>Consolidate spans3</t>
   </si>
 </sst>
 </file>
@@ -466,8 +472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A9F04DC-EF96-45BA-9879-6DBCF76CA793}">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,7 +499,7 @@
         <v>305</v>
       </c>
       <c r="C2" s="1">
-        <f t="shared" ref="C2:C29" si="0">B2/30</f>
+        <f t="shared" ref="C2:C31" si="0">B2/30</f>
         <v>10.166666666666666</v>
       </c>
       <c r="D2" s="2">
@@ -606,7 +612,7 @@
         <v>10.966666666666667</v>
       </c>
       <c r="D9" s="2">
-        <f t="shared" ref="D9:D29" si="2">B9/$B$2</f>
+        <f t="shared" ref="D9:D31" si="2">B9/$B$2</f>
         <v>1.0786885245901638</v>
       </c>
     </row>
@@ -928,6 +934,38 @@
       <c r="D29" s="2">
         <f t="shared" si="2"/>
         <v>1.118032786885246</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30">
+        <v>343</v>
+      </c>
+      <c r="C30" s="1">
+        <f t="shared" si="0"/>
+        <v>11.433333333333334</v>
+      </c>
+      <c r="D30" s="2">
+        <f t="shared" si="2"/>
+        <v>1.1245901639344262</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31">
+        <v>354</v>
+      </c>
+      <c r="C31" s="1">
+        <f t="shared" si="0"/>
+        <v>11.8</v>
+      </c>
+      <c r="D31" s="2">
+        <f t="shared" si="2"/>
+        <v>1.160655737704918</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Per polygon AABB tests. Fix texture quality issues.
</commit_message>
<xml_diff>
--- a/P3DFps.xlsx
+++ b/P3DFps.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zak\Documents\GitProjects\Potato3d\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EA64FBB-2F07-4A91-851B-E3E76AC87BA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7198818-41CF-42A6-B11A-C02C49B7A147}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2904C00D-6B2E-49C9-A39A-1A4D989C3045}"/>
+    <workbookView xWindow="7230" yWindow="480" windowWidth="21570" windowHeight="11370" xr2:uid="{2904C00D-6B2E-49C9-A39A-1A4D989C3045}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
   <si>
     <t>BSP</t>
   </si>
@@ -109,6 +109,30 @@
   </si>
   <si>
     <t>DKR Castle</t>
+  </si>
+  <si>
+    <t>Skip consolidate</t>
+  </si>
+  <si>
+    <t>Skip consolidate 4</t>
+  </si>
+  <si>
+    <t>120*80</t>
+  </si>
+  <si>
+    <t>BB Test polys</t>
+  </si>
+  <si>
+    <t>BB Test polys 2</t>
+  </si>
+  <si>
+    <t>8x unroll</t>
+  </si>
+  <si>
+    <t>No render stats</t>
+  </si>
+  <si>
+    <t>Division factor</t>
   </si>
 </sst>
 </file>
@@ -467,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A9F04DC-EF96-45BA-9879-6DBCF76CA793}">
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -973,11 +997,11 @@
         <v>315</v>
       </c>
       <c r="C33" s="1">
-        <f t="shared" ref="C32:C36" si="3">B33/30</f>
+        <f t="shared" ref="C33:C39" si="3">B33/30</f>
         <v>10.5</v>
       </c>
       <c r="D33" s="2">
-        <f t="shared" ref="D32:D36" si="4">B33/$B$2</f>
+        <f t="shared" ref="D33:D39" si="4">B33/$B$2</f>
         <v>1.0327868852459017</v>
       </c>
     </row>
@@ -1030,10 +1054,212 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="3"/>
+      <c r="A37" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B37">
+        <v>171</v>
+      </c>
+      <c r="C37" s="1">
+        <f t="shared" si="3"/>
+        <v>5.7</v>
+      </c>
+      <c r="D37" s="2">
+        <f t="shared" si="4"/>
+        <v>0.56065573770491806</v>
+      </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="3"/>
+      <c r="A38" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B38">
+        <v>166</v>
+      </c>
+      <c r="C38" s="1">
+        <f t="shared" si="3"/>
+        <v>5.5333333333333332</v>
+      </c>
+      <c r="D38" s="2">
+        <f t="shared" si="4"/>
+        <v>0.54426229508196722</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B39">
+        <v>371</v>
+      </c>
+      <c r="C39" s="1">
+        <f t="shared" si="3"/>
+        <v>12.366666666666667</v>
+      </c>
+      <c r="D39" s="2">
+        <f t="shared" si="4"/>
+        <v>1.2163934426229508</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B41">
+        <v>342</v>
+      </c>
+      <c r="C41" s="1">
+        <f t="shared" ref="C41:C42" si="5">B41/30</f>
+        <v>11.4</v>
+      </c>
+      <c r="D41" s="2">
+        <f t="shared" ref="D41:D42" si="6">B41/$B$2</f>
+        <v>1.1213114754098361</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B42">
+        <v>186</v>
+      </c>
+      <c r="C42" s="1">
+        <f t="shared" si="5"/>
+        <v>6.2</v>
+      </c>
+      <c r="D42" s="2">
+        <f t="shared" si="6"/>
+        <v>0.60983606557377046</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B44">
+        <v>347</v>
+      </c>
+      <c r="C44" s="1">
+        <f t="shared" ref="C44" si="7">B44/30</f>
+        <v>11.566666666666666</v>
+      </c>
+      <c r="D44" s="2">
+        <f t="shared" ref="D44" si="8">B44/$B$2</f>
+        <v>1.1377049180327869</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B45">
+        <v>191</v>
+      </c>
+      <c r="C45" s="1">
+        <f t="shared" ref="C45" si="9">B45/30</f>
+        <v>6.3666666666666663</v>
+      </c>
+      <c r="D45" s="2">
+        <f t="shared" ref="D45" si="10">B45/$B$2</f>
+        <v>0.6262295081967213</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B47">
+        <v>338</v>
+      </c>
+      <c r="C47" s="1">
+        <f t="shared" ref="C47" si="11">B47/30</f>
+        <v>11.266666666666667</v>
+      </c>
+      <c r="D47" s="2">
+        <f t="shared" ref="D47" si="12">B47/$B$2</f>
+        <v>1.1081967213114754</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B48">
+        <v>177</v>
+      </c>
+      <c r="C48" s="1">
+        <f t="shared" ref="C48" si="13">B48/30</f>
+        <v>5.9</v>
+      </c>
+      <c r="D48" s="2">
+        <f t="shared" ref="D48" si="14">B48/$B$2</f>
+        <v>0.58032786885245902</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B50">
+        <v>355</v>
+      </c>
+      <c r="C50" s="1">
+        <f t="shared" ref="C50" si="15">B50/30</f>
+        <v>11.833333333333334</v>
+      </c>
+      <c r="D50" s="2">
+        <f t="shared" ref="D50" si="16">B50/$B$2</f>
+        <v>1.1639344262295082</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B51">
+        <v>235</v>
+      </c>
+      <c r="C51" s="1">
+        <f t="shared" ref="C51" si="17">B51/30</f>
+        <v>7.833333333333333</v>
+      </c>
+      <c r="D51" s="2">
+        <f t="shared" ref="D51" si="18">B51/$B$2</f>
+        <v>0.77049180327868849</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B53">
+        <v>370</v>
+      </c>
+      <c r="C53" s="1">
+        <f t="shared" ref="C52:C54" si="19">B53/30</f>
+        <v>12.333333333333334</v>
+      </c>
+      <c r="D53" s="2">
+        <f t="shared" ref="D52:D54" si="20">B53/$B$2</f>
+        <v>1.2131147540983607</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B54">
+        <v>235</v>
+      </c>
+      <c r="C54" s="1">
+        <f t="shared" si="19"/>
+        <v>7.833333333333333</v>
+      </c>
+      <c r="D54" s="2">
+        <f t="shared" si="20"/>
+        <v>0.77049180327868849</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Prestep UV for quantised pixel coordinates
</commit_message>
<xml_diff>
--- a/P3DFps.xlsx
+++ b/P3DFps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zak\Documents\GitProjects\Potato3d\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FAF1BB2-E3A2-4CA7-9563-30D64A168241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3338E5A0-9F70-445E-9021-D03EE0E21F26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4230" yWindow="2820" windowWidth="21570" windowHeight="11370" xr2:uid="{2904C00D-6B2E-49C9-A39A-1A4D989C3045}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="56">
   <si>
     <t>BSP</t>
   </si>
@@ -187,6 +187,12 @@
   </si>
   <si>
     <t>Unified path</t>
+  </si>
+  <si>
+    <t>Affine Texture</t>
+  </si>
+  <si>
+    <t>No lerp W</t>
   </si>
 </sst>
 </file>
@@ -546,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A9F04DC-EF96-45BA-9879-6DBCF76CA793}">
-  <dimension ref="A1:H94"/>
+  <dimension ref="A1:H96"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="E92" sqref="E92"/>
+      <selection activeCell="A94" sqref="A94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1518,7 +1524,7 @@
         <v>416</v>
       </c>
       <c r="C74" s="1">
-        <f t="shared" ref="C74:C92" si="43">B74/30</f>
+        <f t="shared" ref="C74:C94" si="43">B74/30</f>
         <v>13.866666666666667</v>
       </c>
       <c r="D74" s="2">
@@ -1649,7 +1655,7 @@
         <v>6.8666666666666663</v>
       </c>
       <c r="D87" s="2">
-        <f t="shared" ref="D87:D92" si="47">B87/B$85</f>
+        <f t="shared" ref="D87:D94" si="47">B87/B$85</f>
         <v>1.0618556701030928</v>
       </c>
       <c r="E87">
@@ -1818,19 +1824,49 @@
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G93" s="4"/>
-      <c r="H93" s="4"/>
+      <c r="A93" t="s">
+        <v>54</v>
+      </c>
+      <c r="B93">
+        <v>265</v>
+      </c>
+      <c r="C93" s="1">
+        <f t="shared" si="43"/>
+        <v>8.8333333333333339</v>
+      </c>
+      <c r="D93" s="2">
+        <f t="shared" si="47"/>
+        <v>1.365979381443299</v>
+      </c>
+      <c r="E93">
+        <v>252</v>
+      </c>
+      <c r="F93">
+        <v>909</v>
+      </c>
+      <c r="G93" s="4">
+        <f t="shared" ref="G93" si="50">E93*C93</f>
+        <v>2226</v>
+      </c>
+      <c r="H93" s="4">
+        <f t="shared" ref="H93" si="51">F93*C93</f>
+        <v>8029.5000000000009</v>
+      </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="B94">
-        <v>205</v>
+        <v>274</v>
       </c>
       <c r="C94" s="1">
-        <f t="shared" ref="C94" si="50">B94/30</f>
-        <v>6.833333333333333</v>
+        <f t="shared" si="43"/>
+        <v>9.1333333333333329</v>
+      </c>
+      <c r="D94" s="2">
+        <f t="shared" si="47"/>
+        <v>1.4123711340206186</v>
       </c>
       <c r="E94">
         <v>252</v>
@@ -1839,11 +1875,41 @@
         <v>909</v>
       </c>
       <c r="G94" s="4">
-        <f t="shared" ref="G94" si="51">E94*C94</f>
+        <f t="shared" ref="G94" si="52">E94*C94</f>
+        <v>2301.6</v>
+      </c>
+      <c r="H94" s="4">
+        <f t="shared" ref="H94" si="53">F94*C94</f>
+        <v>8302.1999999999989</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G95" s="4"/>
+      <c r="H95" s="4"/>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>48</v>
+      </c>
+      <c r="B96">
+        <v>205</v>
+      </c>
+      <c r="C96" s="1">
+        <f t="shared" ref="C96" si="54">B96/30</f>
+        <v>6.833333333333333</v>
+      </c>
+      <c r="E96">
+        <v>252</v>
+      </c>
+      <c r="F96">
+        <v>909</v>
+      </c>
+      <c r="G96" s="4">
+        <f t="shared" ref="G96" si="55">E96*C96</f>
         <v>1722</v>
       </c>
-      <c r="H94" s="4">
-        <f t="shared" ref="H94" si="52">F94*C94</f>
+      <c r="H96" s="4">
+        <f t="shared" ref="H96" si="56">F96*C96</f>
         <v>6211.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Combine UV in pixel loop.
</commit_message>
<xml_diff>
--- a/P3DFps.xlsx
+++ b/P3DFps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zak\Documents\GitProjects\Potato3d\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E3DA999-54E4-4601-8FF4-534E8D7F1829}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D84BB16C-E56F-49AF-A93A-D227800BF17C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2904C00D-6B2E-49C9-A39A-1A4D989C3045}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="67">
   <si>
     <t>BSP</t>
   </si>
@@ -202,15 +203,40 @@
   </si>
   <si>
     <t>Vertex Cache</t>
+  </si>
+  <si>
+    <t>Streets</t>
+  </si>
+  <si>
+    <t>Pallete</t>
+  </si>
+  <si>
+    <t>S Def</t>
+  </si>
+  <si>
+    <t>S Buildings</t>
+  </si>
+  <si>
+    <t>b2f</t>
+  </si>
+  <si>
+    <t>f2b</t>
+  </si>
+  <si>
+    <t>Btn Buildings</t>
+  </si>
+  <si>
+    <t>b2f no tex</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -241,12 +267,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -561,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A9F04DC-EF96-45BA-9879-6DBCF76CA793}">
-  <dimension ref="A1:H99"/>
+  <dimension ref="A1:H114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="C97" sqref="C97"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="C115" sqref="C115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1179,11 +1206,11 @@
         <v>342</v>
       </c>
       <c r="C41" s="1">
-        <f t="shared" ref="C41:C42" si="5">B41/30</f>
+        <f>B41/30</f>
         <v>11.4</v>
       </c>
       <c r="D41" s="2">
-        <f t="shared" ref="D41:D42" si="6">B41/$B$2</f>
+        <f>B41/$B$2</f>
         <v>1.1213114754098361</v>
       </c>
     </row>
@@ -1195,11 +1222,11 @@
         <v>186</v>
       </c>
       <c r="C42" s="1">
-        <f t="shared" si="5"/>
+        <f>B42/30</f>
         <v>6.2</v>
       </c>
       <c r="D42" s="2">
-        <f t="shared" si="6"/>
+        <f>B42/$B$2</f>
         <v>0.60983606557377046</v>
       </c>
     </row>
@@ -1211,11 +1238,11 @@
         <v>347</v>
       </c>
       <c r="C44" s="1">
-        <f t="shared" ref="C44" si="7">B44/30</f>
+        <f>B44/30</f>
         <v>11.566666666666666</v>
       </c>
       <c r="D44" s="2">
-        <f t="shared" ref="D44" si="8">B44/$B$2</f>
+        <f>B44/$B$2</f>
         <v>1.1377049180327869</v>
       </c>
     </row>
@@ -1227,11 +1254,11 @@
         <v>191</v>
       </c>
       <c r="C45" s="1">
-        <f t="shared" ref="C45" si="9">B45/30</f>
+        <f>B45/30</f>
         <v>6.3666666666666663</v>
       </c>
       <c r="D45" s="2">
-        <f t="shared" ref="D45" si="10">B45/$B$2</f>
+        <f>B45/$B$2</f>
         <v>0.6262295081967213</v>
       </c>
     </row>
@@ -1243,11 +1270,11 @@
         <v>338</v>
       </c>
       <c r="C47" s="1">
-        <f t="shared" ref="C47" si="11">B47/30</f>
+        <f>B47/30</f>
         <v>11.266666666666667</v>
       </c>
       <c r="D47" s="2">
-        <f t="shared" ref="D47" si="12">B47/$B$2</f>
+        <f>B47/$B$2</f>
         <v>1.1081967213114754</v>
       </c>
     </row>
@@ -1259,11 +1286,11 @@
         <v>177</v>
       </c>
       <c r="C48" s="1">
-        <f t="shared" ref="C48" si="13">B48/30</f>
+        <f>B48/30</f>
         <v>5.9</v>
       </c>
       <c r="D48" s="2">
-        <f t="shared" ref="D48" si="14">B48/$B$2</f>
+        <f>B48/$B$2</f>
         <v>0.58032786885245902</v>
       </c>
     </row>
@@ -1275,11 +1302,11 @@
         <v>355</v>
       </c>
       <c r="C50" s="1">
-        <f t="shared" ref="C50" si="15">B50/30</f>
+        <f>B50/30</f>
         <v>11.833333333333334</v>
       </c>
       <c r="D50" s="2">
-        <f t="shared" ref="D50" si="16">B50/$B$2</f>
+        <f>B50/$B$2</f>
         <v>1.1639344262295082</v>
       </c>
     </row>
@@ -1291,11 +1318,11 @@
         <v>235</v>
       </c>
       <c r="C51" s="1">
-        <f t="shared" ref="C51" si="17">B51/30</f>
+        <f>B51/30</f>
         <v>7.833333333333333</v>
       </c>
       <c r="D51" s="2">
-        <f t="shared" ref="D51" si="18">B51/$B$2</f>
+        <f>B51/$B$2</f>
         <v>0.77049180327868849</v>
       </c>
     </row>
@@ -1307,11 +1334,11 @@
         <v>370</v>
       </c>
       <c r="C53" s="1">
-        <f t="shared" ref="C53:C54" si="19">B53/30</f>
+        <f>B53/30</f>
         <v>12.333333333333334</v>
       </c>
       <c r="D53" s="2">
-        <f t="shared" ref="D53:D54" si="20">B53/$B$2</f>
+        <f>B53/$B$2</f>
         <v>1.2131147540983607</v>
       </c>
     </row>
@@ -1323,11 +1350,11 @@
         <v>235</v>
       </c>
       <c r="C54" s="1">
-        <f t="shared" si="19"/>
+        <f>B54/30</f>
         <v>7.833333333333333</v>
       </c>
       <c r="D54" s="2">
-        <f t="shared" si="20"/>
+        <f>B54/$B$2</f>
         <v>0.77049180327868849</v>
       </c>
     </row>
@@ -1339,11 +1366,11 @@
         <v>405</v>
       </c>
       <c r="C56" s="1">
-        <f t="shared" ref="C56:C57" si="21">B56/30</f>
+        <f>B56/30</f>
         <v>13.5</v>
       </c>
       <c r="D56" s="2">
-        <f t="shared" ref="D56:D57" si="22">B56/$B$2</f>
+        <f>B56/$B$2</f>
         <v>1.3278688524590163</v>
       </c>
     </row>
@@ -1355,11 +1382,11 @@
         <v>208</v>
       </c>
       <c r="C57" s="1">
-        <f t="shared" si="21"/>
+        <f>B57/30</f>
         <v>6.9333333333333336</v>
       </c>
       <c r="D57" s="2">
-        <f t="shared" si="22"/>
+        <f>B57/$B$2</f>
         <v>0.68196721311475406</v>
       </c>
     </row>
@@ -1371,11 +1398,11 @@
         <v>293</v>
       </c>
       <c r="C59" s="1">
-        <f t="shared" ref="C59" si="23">B59/30</f>
+        <f>B59/30</f>
         <v>9.7666666666666675</v>
       </c>
       <c r="D59" s="2">
-        <f t="shared" ref="D59" si="24">B59/$B$2</f>
+        <f>B59/$B$2</f>
         <v>0.96065573770491808</v>
       </c>
     </row>
@@ -1387,11 +1414,11 @@
         <v>401</v>
       </c>
       <c r="C61" s="1">
-        <f t="shared" ref="C61" si="25">B61/30</f>
+        <f>B61/30</f>
         <v>13.366666666666667</v>
       </c>
       <c r="D61" s="2">
-        <f t="shared" ref="D61" si="26">B61/$B$2</f>
+        <f>B61/$B$2</f>
         <v>1.3147540983606558</v>
       </c>
     </row>
@@ -1403,11 +1430,11 @@
         <v>212</v>
       </c>
       <c r="C62" s="1">
-        <f t="shared" ref="C62" si="27">B62/30</f>
+        <f>B62/30</f>
         <v>7.0666666666666664</v>
       </c>
       <c r="D62" s="2">
-        <f t="shared" ref="D62" si="28">B62/$B$2</f>
+        <f>B62/$B$2</f>
         <v>0.69508196721311477</v>
       </c>
     </row>
@@ -1419,11 +1446,11 @@
         <v>478</v>
       </c>
       <c r="C64" s="1">
-        <f t="shared" ref="C64" si="29">B64/30</f>
+        <f>B64/30</f>
         <v>15.933333333333334</v>
       </c>
       <c r="D64" s="2">
-        <f t="shared" ref="D64" si="30">B64/$B$2</f>
+        <f>B64/$B$2</f>
         <v>1.5672131147540984</v>
       </c>
     </row>
@@ -1435,11 +1462,11 @@
         <v>223</v>
       </c>
       <c r="C65" s="1">
-        <f t="shared" ref="C65" si="31">B65/30</f>
+        <f>B65/30</f>
         <v>7.4333333333333336</v>
       </c>
       <c r="D65" s="2">
-        <f t="shared" ref="D65" si="32">B65/$B$2</f>
+        <f>B65/$B$2</f>
         <v>0.73114754098360657</v>
       </c>
     </row>
@@ -1451,11 +1478,11 @@
         <v>486</v>
       </c>
       <c r="C67" s="1">
-        <f t="shared" ref="C67" si="33">B67/30</f>
+        <f>B67/30</f>
         <v>16.2</v>
       </c>
       <c r="D67" s="2">
-        <f t="shared" ref="D67" si="34">B67/$B$2</f>
+        <f>B67/$B$2</f>
         <v>1.5934426229508196</v>
       </c>
     </row>
@@ -1467,11 +1494,11 @@
         <v>198</v>
       </c>
       <c r="C68" s="1">
-        <f t="shared" ref="C68" si="35">B68/30</f>
+        <f>B68/30</f>
         <v>6.6</v>
       </c>
       <c r="D68" s="2">
-        <f t="shared" ref="D68" si="36">B68/$B$2</f>
+        <f>B68/$B$2</f>
         <v>0.64918032786885249</v>
       </c>
     </row>
@@ -1483,11 +1510,11 @@
         <v>312</v>
       </c>
       <c r="C70" s="1">
-        <f t="shared" ref="C70" si="37">B70/30</f>
+        <f>B70/30</f>
         <v>10.4</v>
       </c>
       <c r="D70" s="2">
-        <f t="shared" ref="D70" si="38">B70/$B$2</f>
+        <f>B70/$B$2</f>
         <v>1.0229508196721311</v>
       </c>
       <c r="G70" s="1"/>
@@ -1501,11 +1528,11 @@
         <v>403</v>
       </c>
       <c r="C71" s="1">
-        <f t="shared" ref="C71" si="39">B71/30</f>
+        <f>B71/30</f>
         <v>13.433333333333334</v>
       </c>
       <c r="D71" s="2">
-        <f t="shared" ref="D71" si="40">B71/$B$2</f>
+        <f>B71/$B$2</f>
         <v>1.3213114754098361</v>
       </c>
     </row>
@@ -1517,11 +1544,11 @@
         <v>710</v>
       </c>
       <c r="C73" s="1">
-        <f t="shared" ref="C73" si="41">B73/30</f>
+        <f>B73/30</f>
         <v>23.666666666666668</v>
       </c>
       <c r="D73" s="2">
-        <f t="shared" ref="D73" si="42">B73/$B$2</f>
+        <f>B73/$B$2</f>
         <v>2.3278688524590163</v>
       </c>
     </row>
@@ -1533,11 +1560,11 @@
         <v>416</v>
       </c>
       <c r="C74" s="1">
-        <f t="shared" ref="C74:C97" si="43">B74/30</f>
+        <f t="shared" ref="C74:C97" si="5">B74/30</f>
         <v>13.866666666666667</v>
       </c>
       <c r="D74" s="2">
-        <f t="shared" ref="D74" si="44">B74/$B$2</f>
+        <f>B74/$B$2</f>
         <v>1.3639344262295081</v>
       </c>
     </row>
@@ -1549,7 +1576,7 @@
         <v>371</v>
       </c>
       <c r="C77" s="1">
-        <f t="shared" si="43"/>
+        <f t="shared" si="5"/>
         <v>12.366666666666667</v>
       </c>
     </row>
@@ -1561,7 +1588,7 @@
         <v>343</v>
       </c>
       <c r="C78" s="1">
-        <f t="shared" si="43"/>
+        <f t="shared" si="5"/>
         <v>11.433333333333334</v>
       </c>
     </row>
@@ -1573,7 +1600,7 @@
         <v>341</v>
       </c>
       <c r="C79" s="1">
-        <f t="shared" si="43"/>
+        <f t="shared" si="5"/>
         <v>11.366666666666667</v>
       </c>
     </row>
@@ -1582,7 +1609,7 @@
         <v>170</v>
       </c>
       <c r="C81" s="1">
-        <f t="shared" si="43"/>
+        <f t="shared" si="5"/>
         <v>5.666666666666667</v>
       </c>
     </row>
@@ -1591,7 +1618,7 @@
         <v>127</v>
       </c>
       <c r="C82" s="1">
-        <f t="shared" si="43"/>
+        <f t="shared" si="5"/>
         <v>4.2333333333333334</v>
       </c>
     </row>
@@ -1600,7 +1627,7 @@
         <v>194</v>
       </c>
       <c r="C85" s="1">
-        <f t="shared" si="43"/>
+        <f t="shared" si="5"/>
         <v>6.4666666666666668</v>
       </c>
       <c r="D85" s="2">
@@ -1614,11 +1641,11 @@
         <v>909</v>
       </c>
       <c r="G85" s="4">
-        <f t="shared" ref="G85:G91" si="45">E85*C85</f>
+        <f t="shared" ref="G85:G91" si="6">E85*C85</f>
         <v>1629.6000000000001</v>
       </c>
       <c r="H85" s="4">
-        <f t="shared" ref="H85:H91" si="46">F85*C85</f>
+        <f t="shared" ref="H85:H91" si="7">F85*C85</f>
         <v>5878.2</v>
       </c>
     </row>
@@ -1630,7 +1657,7 @@
         <v>199</v>
       </c>
       <c r="C86" s="1">
-        <f t="shared" si="43"/>
+        <f t="shared" si="5"/>
         <v>6.6333333333333337</v>
       </c>
       <c r="D86" s="2">
@@ -1644,11 +1671,11 @@
         <v>909</v>
       </c>
       <c r="G86" s="4">
-        <f t="shared" si="45"/>
+        <f t="shared" si="6"/>
         <v>1671.6000000000001</v>
       </c>
       <c r="H86" s="4">
-        <f t="shared" si="46"/>
+        <f t="shared" si="7"/>
         <v>6029.7000000000007</v>
       </c>
     </row>
@@ -1660,11 +1687,11 @@
         <v>206</v>
       </c>
       <c r="C87" s="1">
-        <f t="shared" si="43"/>
+        <f t="shared" si="5"/>
         <v>6.8666666666666663</v>
       </c>
       <c r="D87" s="2">
-        <f t="shared" ref="D87:D97" si="47">B87/B$85</f>
+        <f t="shared" ref="D87:D97" si="8">B87/B$85</f>
         <v>1.0618556701030928</v>
       </c>
       <c r="E87">
@@ -1674,11 +1701,11 @@
         <v>909</v>
       </c>
       <c r="G87" s="4">
-        <f t="shared" si="45"/>
+        <f t="shared" si="6"/>
         <v>1730.3999999999999</v>
       </c>
       <c r="H87" s="4">
-        <f t="shared" si="46"/>
+        <f t="shared" si="7"/>
         <v>6241.7999999999993</v>
       </c>
     </row>
@@ -1690,11 +1717,11 @@
         <v>208</v>
       </c>
       <c r="C88" s="1">
-        <f t="shared" si="43"/>
+        <f t="shared" si="5"/>
         <v>6.9333333333333336</v>
       </c>
       <c r="D88" s="2">
-        <f t="shared" si="47"/>
+        <f t="shared" si="8"/>
         <v>1.0721649484536082</v>
       </c>
       <c r="E88">
@@ -1704,11 +1731,11 @@
         <v>909</v>
       </c>
       <c r="G88" s="4">
-        <f t="shared" si="45"/>
+        <f t="shared" si="6"/>
         <v>1747.2</v>
       </c>
       <c r="H88" s="4">
-        <f t="shared" si="46"/>
+        <f t="shared" si="7"/>
         <v>6302.4000000000005</v>
       </c>
     </row>
@@ -1720,11 +1747,11 @@
         <v>207</v>
       </c>
       <c r="C89" s="1">
-        <f t="shared" si="43"/>
+        <f t="shared" si="5"/>
         <v>6.9</v>
       </c>
       <c r="D89" s="2">
-        <f t="shared" si="47"/>
+        <f t="shared" si="8"/>
         <v>1.0670103092783505</v>
       </c>
       <c r="E89">
@@ -1734,11 +1761,11 @@
         <v>909</v>
       </c>
       <c r="G89" s="4">
-        <f t="shared" si="45"/>
+        <f t="shared" si="6"/>
         <v>1738.8000000000002</v>
       </c>
       <c r="H89" s="4">
-        <f t="shared" si="46"/>
+        <f t="shared" si="7"/>
         <v>6272.1</v>
       </c>
     </row>
@@ -1750,11 +1777,11 @@
         <v>209</v>
       </c>
       <c r="C90" s="1">
-        <f t="shared" si="43"/>
+        <f t="shared" si="5"/>
         <v>6.9666666666666668</v>
       </c>
       <c r="D90" s="2">
-        <f t="shared" si="47"/>
+        <f t="shared" si="8"/>
         <v>1.0773195876288659</v>
       </c>
       <c r="E90">
@@ -1764,11 +1791,11 @@
         <v>909</v>
       </c>
       <c r="G90" s="4">
-        <f t="shared" si="45"/>
+        <f t="shared" si="6"/>
         <v>1755.6000000000001</v>
       </c>
       <c r="H90" s="4">
-        <f t="shared" si="46"/>
+        <f t="shared" si="7"/>
         <v>6332.7</v>
       </c>
     </row>
@@ -1780,11 +1807,11 @@
         <v>237</v>
       </c>
       <c r="C91" s="1">
-        <f t="shared" si="43"/>
+        <f t="shared" si="5"/>
         <v>7.9</v>
       </c>
       <c r="D91" s="2">
-        <f t="shared" si="47"/>
+        <f t="shared" si="8"/>
         <v>1.2216494845360826</v>
       </c>
       <c r="E91">
@@ -1794,11 +1821,11 @@
         <v>909</v>
       </c>
       <c r="G91" s="4">
-        <f t="shared" si="45"/>
+        <f t="shared" si="6"/>
         <v>1990.8000000000002</v>
       </c>
       <c r="H91" s="4">
-        <f t="shared" si="46"/>
+        <f t="shared" si="7"/>
         <v>7181.1</v>
       </c>
     </row>
@@ -1810,11 +1837,11 @@
         <v>234</v>
       </c>
       <c r="C92" s="1">
-        <f t="shared" si="43"/>
+        <f t="shared" si="5"/>
         <v>7.8</v>
       </c>
       <c r="D92" s="2">
-        <f t="shared" si="47"/>
+        <f t="shared" si="8"/>
         <v>1.2061855670103092</v>
       </c>
       <c r="E92">
@@ -1824,11 +1851,11 @@
         <v>909</v>
       </c>
       <c r="G92" s="4">
-        <f t="shared" ref="G92" si="48">E92*C92</f>
+        <f t="shared" ref="G92:G97" si="9">E92*C92</f>
         <v>1965.6</v>
       </c>
       <c r="H92" s="4">
-        <f t="shared" ref="H92" si="49">F92*C92</f>
+        <f t="shared" ref="H92:H97" si="10">F92*C92</f>
         <v>7090.2</v>
       </c>
     </row>
@@ -1840,11 +1867,11 @@
         <v>265</v>
       </c>
       <c r="C93" s="1">
-        <f t="shared" si="43"/>
+        <f t="shared" si="5"/>
         <v>8.8333333333333339</v>
       </c>
       <c r="D93" s="2">
-        <f t="shared" si="47"/>
+        <f t="shared" si="8"/>
         <v>1.365979381443299</v>
       </c>
       <c r="E93">
@@ -1854,11 +1881,11 @@
         <v>909</v>
       </c>
       <c r="G93" s="4">
-        <f t="shared" ref="G93" si="50">E93*C93</f>
+        <f t="shared" si="9"/>
         <v>2226</v>
       </c>
       <c r="H93" s="4">
-        <f t="shared" ref="H93" si="51">F93*C93</f>
+        <f t="shared" si="10"/>
         <v>8029.5000000000009</v>
       </c>
     </row>
@@ -1870,11 +1897,11 @@
         <v>274</v>
       </c>
       <c r="C94" s="1">
-        <f t="shared" si="43"/>
+        <f t="shared" si="5"/>
         <v>9.1333333333333329</v>
       </c>
       <c r="D94" s="2">
-        <f t="shared" si="47"/>
+        <f t="shared" si="8"/>
         <v>1.4123711340206186</v>
       </c>
       <c r="E94">
@@ -1884,11 +1911,11 @@
         <v>909</v>
       </c>
       <c r="G94" s="4">
-        <f t="shared" ref="G94" si="52">E94*C94</f>
+        <f t="shared" si="9"/>
         <v>2301.6</v>
       </c>
       <c r="H94" s="4">
-        <f t="shared" ref="H94" si="53">F94*C94</f>
+        <f t="shared" si="10"/>
         <v>8302.1999999999989</v>
       </c>
     </row>
@@ -1900,11 +1927,11 @@
         <v>272</v>
       </c>
       <c r="C95" s="1">
-        <f t="shared" si="43"/>
+        <f t="shared" si="5"/>
         <v>9.0666666666666664</v>
       </c>
       <c r="D95" s="2">
-        <f t="shared" si="47"/>
+        <f t="shared" si="8"/>
         <v>1.402061855670103</v>
       </c>
       <c r="E95">
@@ -1914,11 +1941,11 @@
         <v>910</v>
       </c>
       <c r="G95" s="4">
-        <f t="shared" ref="G95" si="54">E95*C95</f>
+        <f t="shared" si="9"/>
         <v>2284.7999999999997</v>
       </c>
       <c r="H95" s="4">
-        <f t="shared" ref="H95" si="55">F95*C95</f>
+        <f t="shared" si="10"/>
         <v>8250.6666666666661</v>
       </c>
     </row>
@@ -1930,11 +1957,11 @@
         <v>284</v>
       </c>
       <c r="C96" s="1">
-        <f t="shared" si="43"/>
+        <f t="shared" si="5"/>
         <v>9.4666666666666668</v>
       </c>
       <c r="D96" s="2">
-        <f t="shared" si="47"/>
+        <f t="shared" si="8"/>
         <v>1.4639175257731958</v>
       </c>
       <c r="E96">
@@ -1944,11 +1971,11 @@
         <v>910</v>
       </c>
       <c r="G96" s="4">
-        <f t="shared" ref="G96" si="56">E96*C96</f>
+        <f t="shared" si="9"/>
         <v>2385.6</v>
       </c>
       <c r="H96" s="4">
-        <f t="shared" ref="H96" si="57">F96*C96</f>
+        <f t="shared" si="10"/>
         <v>8614.6666666666661</v>
       </c>
     </row>
@@ -1960,11 +1987,11 @@
         <v>296</v>
       </c>
       <c r="C97" s="1">
-        <f t="shared" si="43"/>
+        <f t="shared" si="5"/>
         <v>9.8666666666666671</v>
       </c>
       <c r="D97" s="2">
-        <f t="shared" si="47"/>
+        <f t="shared" si="8"/>
         <v>1.5257731958762886</v>
       </c>
       <c r="E97">
@@ -1974,42 +2001,245 @@
         <v>910</v>
       </c>
       <c r="G97" s="4">
-        <f t="shared" ref="G97" si="58">E97*C97</f>
+        <f t="shared" si="9"/>
         <v>2486.4</v>
       </c>
       <c r="H97" s="4">
-        <f t="shared" ref="H97" si="59">F97*C97</f>
+        <f t="shared" si="10"/>
         <v>8978.6666666666679</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G98" s="4"/>
-      <c r="H98" s="4"/>
+      <c r="A98" t="s">
+        <v>60</v>
+      </c>
+      <c r="B98">
+        <v>280</v>
+      </c>
+      <c r="C98" s="1">
+        <f t="shared" ref="C98" si="11">B98/30</f>
+        <v>9.3333333333333339</v>
+      </c>
+      <c r="D98" s="2">
+        <f t="shared" ref="D98:D99" si="12">B98/B$85</f>
+        <v>1.4432989690721649</v>
+      </c>
+      <c r="E98">
+        <v>273</v>
+      </c>
+      <c r="F98">
+        <v>910</v>
+      </c>
+      <c r="G98" s="4">
+        <f t="shared" ref="G98" si="13">E98*C98</f>
+        <v>2548</v>
+      </c>
+      <c r="H98" s="4">
+        <f t="shared" ref="H98" si="14">F98*C98</f>
+        <v>8493.3333333333339</v>
+      </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>48</v>
       </c>
       <c r="B99">
-        <v>205</v>
+        <v>315</v>
       </c>
       <c r="C99" s="1">
-        <f t="shared" ref="C99" si="60">B99/30</f>
-        <v>6.833333333333333</v>
+        <f>B99/30</f>
+        <v>10.5</v>
+      </c>
+      <c r="D99" s="2">
+        <f t="shared" si="12"/>
+        <v>1.6237113402061856</v>
       </c>
       <c r="E99">
-        <v>252</v>
+        <v>273</v>
       </c>
       <c r="F99">
         <v>909</v>
       </c>
       <c r="G99" s="4">
-        <f t="shared" ref="G99" si="61">E99*C99</f>
-        <v>1722</v>
+        <f>E99*C99</f>
+        <v>2866.5</v>
       </c>
       <c r="H99" s="4">
-        <f t="shared" ref="H99" si="62">F99*C99</f>
-        <v>6211.5</v>
+        <f>F99*C99</f>
+        <v>9544.5</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G100" s="4"/>
+      <c r="H100" s="4"/>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>59</v>
+      </c>
+      <c r="B101">
+        <v>356</v>
+      </c>
+      <c r="C101" s="1">
+        <f>B101/30</f>
+        <v>11.866666666666667</v>
+      </c>
+      <c r="E101">
+        <v>252</v>
+      </c>
+      <c r="F101">
+        <v>909</v>
+      </c>
+      <c r="G101" s="4">
+        <f>E101*C101</f>
+        <v>2990.4</v>
+      </c>
+      <c r="H101" s="4">
+        <f>F101*C101</f>
+        <v>10786.800000000001</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B105" t="s">
+        <v>63</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>61</v>
+      </c>
+      <c r="B106">
+        <v>551</v>
+      </c>
+      <c r="C106" s="1">
+        <v>504</v>
+      </c>
+      <c r="D106" s="3">
+        <v>695</v>
+      </c>
+      <c r="E106" s="5">
+        <f>B106/30</f>
+        <v>18.366666666666667</v>
+      </c>
+      <c r="F106" s="5">
+        <f>C106/30</f>
+        <v>16.8</v>
+      </c>
+      <c r="G106" s="5">
+        <f>D106/30</f>
+        <v>23.166666666666668</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>62</v>
+      </c>
+      <c r="B107">
+        <v>334</v>
+      </c>
+      <c r="C107" s="1">
+        <v>255</v>
+      </c>
+      <c r="D107" s="3">
+        <v>468</v>
+      </c>
+      <c r="E107" s="5">
+        <f>B107/30</f>
+        <v>11.133333333333333</v>
+      </c>
+      <c r="F107" s="5">
+        <f>C107/30</f>
+        <v>8.5</v>
+      </c>
+      <c r="G107" s="5">
+        <f>D107/30</f>
+        <v>15.6</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>65</v>
+      </c>
+      <c r="B108">
+        <v>276</v>
+      </c>
+      <c r="C108" s="1">
+        <v>230</v>
+      </c>
+      <c r="D108" s="3">
+        <v>456</v>
+      </c>
+      <c r="E108" s="5">
+        <f>B108/30</f>
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="F108" s="5">
+        <f>C108/30</f>
+        <v>7.666666666666667</v>
+      </c>
+      <c r="G108" s="5">
+        <f>D108/30</f>
+        <v>15.2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E109" s="5"/>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E110" s="5"/>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E111" s="5"/>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>61</v>
+      </c>
+      <c r="B112">
+        <v>561</v>
+      </c>
+      <c r="C112" s="1">
+        <v>561</v>
+      </c>
+      <c r="E112" s="5">
+        <f t="shared" ref="E109:E114" si="15">B112/30</f>
+        <v>18.7</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>62</v>
+      </c>
+      <c r="B113">
+        <v>317</v>
+      </c>
+      <c r="C113" s="1">
+        <v>314</v>
+      </c>
+      <c r="E113" s="5">
+        <f t="shared" si="15"/>
+        <v>10.566666666666666</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>65</v>
+      </c>
+      <c r="B114">
+        <v>295</v>
+      </c>
+      <c r="C114" s="1">
+        <v>291</v>
+      </c>
+      <c r="E114" s="5">
+        <f t="shared" si="15"/>
+        <v>9.8333333333333339</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Only clip if needed.
</commit_message>
<xml_diff>
--- a/P3DFps.xlsx
+++ b/P3DFps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zak\Documents\GitProjects\Potato3d\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D3511F-AF33-416F-A3A8-FDC2C59D6481}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{828EF476-F7D3-4D90-864E-4F414DB8B029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2904C00D-6B2E-49C9-A39A-1A4D989C3045}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="73">
   <si>
     <t>BSP</t>
   </si>
@@ -239,6 +239,12 @@
   </si>
   <si>
     <t>VxPool</t>
+  </si>
+  <si>
+    <t>240x160</t>
+  </si>
+  <si>
+    <t>Ofast</t>
   </si>
 </sst>
 </file>
@@ -600,10 +606,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A9F04DC-EF96-45BA-9879-6DBCF76CA793}">
-  <dimension ref="A1:H126"/>
+  <dimension ref="A1:H138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="D126" sqref="D126"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="B138" sqref="B138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2029,11 +2035,11 @@
         <v>280</v>
       </c>
       <c r="C98" s="1">
-        <f t="shared" ref="C98" si="11">B98/30</f>
+        <f>B98/30</f>
         <v>9.3333333333333339</v>
       </c>
       <c r="D98" s="2">
-        <f t="shared" ref="D98:D99" si="12">B98/B$85</f>
+        <f>B98/B$85</f>
         <v>1.4432989690721649</v>
       </c>
       <c r="E98">
@@ -2043,11 +2049,11 @@
         <v>910</v>
       </c>
       <c r="G98" s="4">
-        <f t="shared" ref="G98" si="13">E98*C98</f>
+        <f>E98*C98</f>
         <v>2548</v>
       </c>
       <c r="H98" s="4">
-        <f t="shared" ref="H98" si="14">F98*C98</f>
+        <f>F98*C98</f>
         <v>8493.3333333333339</v>
       </c>
     </row>
@@ -2063,7 +2069,7 @@
         <v>10.5</v>
       </c>
       <c r="D99" s="2">
-        <f t="shared" si="12"/>
+        <f>B99/B$85</f>
         <v>1.6237113402061856</v>
       </c>
       <c r="E99">
@@ -2136,15 +2142,15 @@
         <v>695</v>
       </c>
       <c r="E106" s="5">
-        <f>B106/30</f>
+        <f t="shared" ref="E106:G108" si="11">B106/30</f>
         <v>18.366666666666667</v>
       </c>
       <c r="F106" s="5">
-        <f>C106/30</f>
+        <f t="shared" si="11"/>
         <v>16.8</v>
       </c>
       <c r="G106" s="5">
-        <f>D106/30</f>
+        <f t="shared" si="11"/>
         <v>23.166666666666668</v>
       </c>
     </row>
@@ -2162,15 +2168,15 @@
         <v>468</v>
       </c>
       <c r="E107" s="5">
-        <f>B107/30</f>
+        <f t="shared" si="11"/>
         <v>11.133333333333333</v>
       </c>
       <c r="F107" s="5">
-        <f>C107/30</f>
+        <f t="shared" si="11"/>
         <v>8.5</v>
       </c>
       <c r="G107" s="5">
-        <f>D107/30</f>
+        <f t="shared" si="11"/>
         <v>15.6</v>
       </c>
     </row>
@@ -2188,15 +2194,15 @@
         <v>456</v>
       </c>
       <c r="E108" s="5">
-        <f>B108/30</f>
+        <f t="shared" si="11"/>
         <v>9.1999999999999993</v>
       </c>
       <c r="F108" s="5">
-        <f>C108/30</f>
+        <f t="shared" si="11"/>
         <v>7.666666666666667</v>
       </c>
       <c r="G108" s="5">
-        <f>D108/30</f>
+        <f t="shared" si="11"/>
         <v>15.2</v>
       </c>
     </row>
@@ -2220,15 +2226,15 @@
         <v>561</v>
       </c>
       <c r="E112" s="5">
-        <f t="shared" ref="E109:F124" si="15">B112/30</f>
+        <f t="shared" ref="E112:F124" si="12">B112/30</f>
         <v>18.7</v>
       </c>
       <c r="F112" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="12"/>
         <v>18.7</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>62</v>
       </c>
@@ -2239,15 +2245,15 @@
         <v>314</v>
       </c>
       <c r="E113" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="12"/>
         <v>10.566666666666666</v>
       </c>
       <c r="F113" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="12"/>
         <v>10.466666666666667</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>65</v>
       </c>
@@ -2258,24 +2264,24 @@
         <v>291</v>
       </c>
       <c r="E114" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="12"/>
         <v>9.8333333333333339</v>
       </c>
       <c r="F114" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="12"/>
         <v>9.6999999999999993</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E115" s="5"/>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>67</v>
       </c>
       <c r="E116" s="5"/>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>61</v>
       </c>
@@ -2286,15 +2292,15 @@
         <v>554</v>
       </c>
       <c r="E117" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="12"/>
         <v>18.433333333333334</v>
       </c>
       <c r="F117" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="12"/>
         <v>18.466666666666665</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>62</v>
       </c>
@@ -2305,15 +2311,15 @@
         <v>317</v>
       </c>
       <c r="E118" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="12"/>
         <v>10.366666666666667</v>
       </c>
       <c r="F118" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="12"/>
         <v>10.566666666666666</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>65</v>
       </c>
@@ -2324,19 +2330,19 @@
         <v>288</v>
       </c>
       <c r="E119" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="12"/>
         <v>9.7333333333333325</v>
       </c>
       <c r="F119" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="12"/>
         <v>9.6</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E120" s="5"/>
       <c r="F120" s="5"/>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>68</v>
       </c>
@@ -2344,12 +2350,12 @@
         <v>381</v>
       </c>
       <c r="E121" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="12"/>
         <v>12.7</v>
       </c>
       <c r="F121" s="5"/>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>69</v>
       </c>
@@ -2357,16 +2363,16 @@
         <v>375</v>
       </c>
       <c r="E122" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="12"/>
         <v>12.5</v>
       </c>
       <c r="F122" s="5"/>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E123" s="5"/>
       <c r="F123" s="5"/>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>70</v>
       </c>
@@ -2377,15 +2383,19 @@
         <v>521</v>
       </c>
       <c r="E124" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="12"/>
         <v>18.266666666666666</v>
       </c>
       <c r="F124" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="12"/>
         <v>17.366666666666667</v>
       </c>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H124" s="2">
+        <f>B124/C124</f>
+        <v>1.051823416506718</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B125">
         <v>309</v>
       </c>
@@ -2393,15 +2403,19 @@
         <v>305</v>
       </c>
       <c r="E125" s="5">
-        <f t="shared" ref="E125:F126" si="16">B125/30</f>
+        <f t="shared" ref="E125:F136" si="13">B125/30</f>
         <v>10.3</v>
       </c>
       <c r="F125" s="5">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v>10.166666666666666</v>
       </c>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H125" s="2">
+        <f>B125/C125</f>
+        <v>1.0131147540983607</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B126">
         <v>292</v>
       </c>
@@ -2409,12 +2423,118 @@
         <v>291</v>
       </c>
       <c r="E126" s="5">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v>9.7333333333333325</v>
       </c>
       <c r="F126" s="5">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v>9.6999999999999993</v>
+      </c>
+      <c r="H126" s="2">
+        <f>B126/C126</f>
+        <v>1.0034364261168385</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E127" s="5"/>
+      <c r="F127" s="5"/>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E128" s="5"/>
+      <c r="F128" s="5"/>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>71</v>
+      </c>
+      <c r="B129">
+        <v>523</v>
+      </c>
+      <c r="E129" s="5">
+        <f t="shared" si="13"/>
+        <v>17.433333333333334</v>
+      </c>
+      <c r="F129" s="5"/>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B130">
+        <v>288</v>
+      </c>
+      <c r="E130" s="5">
+        <f t="shared" si="13"/>
+        <v>9.6</v>
+      </c>
+      <c r="F130" s="5"/>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B131">
+        <v>258</v>
+      </c>
+      <c r="E131" s="5">
+        <f t="shared" si="13"/>
+        <v>8.6</v>
+      </c>
+      <c r="F131" s="5"/>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E132" s="5"/>
+      <c r="F132" s="5"/>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E133" s="5"/>
+      <c r="F133" s="5"/>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B134">
+        <v>402</v>
+      </c>
+      <c r="C134" s="1">
+        <v>435</v>
+      </c>
+      <c r="E134" s="5">
+        <f t="shared" si="13"/>
+        <v>13.4</v>
+      </c>
+      <c r="F134" s="5">
+        <f t="shared" si="13"/>
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B135">
+        <v>225</v>
+      </c>
+      <c r="C135" s="1">
+        <v>268</v>
+      </c>
+      <c r="E135" s="5">
+        <f t="shared" si="13"/>
+        <v>7.5</v>
+      </c>
+      <c r="F135" s="5">
+        <f t="shared" si="13"/>
+        <v>8.9333333333333336</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B136">
+        <v>206</v>
+      </c>
+      <c r="C136" s="1">
+        <v>226</v>
+      </c>
+      <c r="E136" s="5">
+        <f t="shared" si="13"/>
+        <v>6.8666666666666663</v>
+      </c>
+      <c r="F136" s="5">
+        <f t="shared" si="13"/>
+        <v>7.5333333333333332</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reuse clip vx count.
</commit_message>
<xml_diff>
--- a/P3DFps.xlsx
+++ b/P3DFps.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zak\Documents\GitProjects\Potato3d\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{828EF476-F7D3-4D90-864E-4F414DB8B029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC4B2BA7-09E7-4E0A-95E8-C2B9B1370944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2904C00D-6B2E-49C9-A39A-1A4D989C3045}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="80">
   <si>
     <t>BSP</t>
   </si>
@@ -244,7 +244,28 @@
     <t>240x160</t>
   </si>
   <si>
-    <t>Ofast</t>
+    <t>No Right bottom clip</t>
+  </si>
+  <si>
+    <t>Selective Clip</t>
+  </si>
+  <si>
+    <t>Selective Clip2</t>
+  </si>
+  <si>
+    <t>IWRAM</t>
+  </si>
+  <si>
+    <t>Obj3d in IWRAM</t>
+  </si>
+  <si>
+    <t>Z Far clip</t>
+  </si>
+  <si>
+    <t>Skip clip</t>
+  </si>
+  <si>
+    <t>240X160</t>
   </si>
 </sst>
 </file>
@@ -606,10 +627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A9F04DC-EF96-45BA-9879-6DBCF76CA793}">
-  <dimension ref="A1:H138"/>
+  <dimension ref="A1:H162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="B138" sqref="B138"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="F100" sqref="F100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2088,127 +2109,154 @@
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G100" s="4"/>
-      <c r="H100" s="4"/>
+      <c r="A100" t="s">
+        <v>79</v>
+      </c>
+      <c r="B100">
+        <v>308</v>
+      </c>
+      <c r="C100" s="1">
+        <f>B100/30</f>
+        <v>10.266666666666667</v>
+      </c>
+      <c r="D100" s="2">
+        <f>B100/B$85</f>
+        <v>1.5876288659793814</v>
+      </c>
+      <c r="E100">
+        <v>304</v>
+      </c>
+      <c r="F100">
+        <v>294</v>
+      </c>
+      <c r="G100" s="4">
+        <f>E100*C100</f>
+        <v>3121.0666666666671</v>
+      </c>
+      <c r="H100" s="4">
+        <f>F100*C100</f>
+        <v>3018.4</v>
+      </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
+      <c r="G101" s="4"/>
+      <c r="H101" s="4"/>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
         <v>59</v>
       </c>
-      <c r="B101">
+      <c r="B102">
         <v>356</v>
       </c>
-      <c r="C101" s="1">
-        <f>B101/30</f>
+      <c r="C102" s="1">
+        <f>B102/30</f>
         <v>11.866666666666667</v>
       </c>
-      <c r="E101">
+      <c r="E102">
         <v>252</v>
       </c>
-      <c r="F101">
+      <c r="F102">
         <v>909</v>
       </c>
-      <c r="G101" s="4">
-        <f>E101*C101</f>
+      <c r="G102" s="4">
+        <f>E102*C102</f>
         <v>2990.4</v>
       </c>
-      <c r="H101" s="4">
-        <f>F101*C101</f>
+      <c r="H102" s="4">
+        <f>F102*C102</f>
         <v>10786.800000000001</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B105" t="s">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B106" t="s">
         <v>63</v>
       </c>
-      <c r="C105" s="1" t="s">
+      <c r="C106" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D105" s="2" t="s">
+      <c r="D106" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
         <v>61</v>
       </c>
-      <c r="B106">
+      <c r="B107">
         <v>551</v>
       </c>
-      <c r="C106" s="1">
+      <c r="C107" s="1">
         <v>504</v>
       </c>
-      <c r="D106" s="3">
+      <c r="D107" s="3">
         <v>695</v>
       </c>
-      <c r="E106" s="5">
-        <f t="shared" ref="E106:G108" si="11">B106/30</f>
+      <c r="E107" s="5">
+        <f t="shared" ref="E107:G109" si="11">B107/30</f>
         <v>18.366666666666667</v>
       </c>
-      <c r="F106" s="5">
+      <c r="F107" s="5">
         <f t="shared" si="11"/>
         <v>16.8</v>
       </c>
-      <c r="G106" s="5">
+      <c r="G107" s="5">
         <f t="shared" si="11"/>
         <v>23.166666666666668</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
         <v>62</v>
       </c>
-      <c r="B107">
+      <c r="B108">
         <v>334</v>
       </c>
-      <c r="C107" s="1">
+      <c r="C108" s="1">
         <v>255</v>
       </c>
-      <c r="D107" s="3">
+      <c r="D108" s="3">
         <v>468</v>
       </c>
-      <c r="E107" s="5">
+      <c r="E108" s="5">
         <f t="shared" si="11"/>
         <v>11.133333333333333</v>
       </c>
-      <c r="F107" s="5">
+      <c r="F108" s="5">
         <f t="shared" si="11"/>
         <v>8.5</v>
       </c>
-      <c r="G107" s="5">
+      <c r="G108" s="5">
         <f t="shared" si="11"/>
         <v>15.6</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
         <v>65</v>
       </c>
-      <c r="B108">
+      <c r="B109">
         <v>276</v>
       </c>
-      <c r="C108" s="1">
+      <c r="C109" s="1">
         <v>230</v>
       </c>
-      <c r="D108" s="3">
+      <c r="D109" s="3">
         <v>456</v>
       </c>
-      <c r="E108" s="5">
+      <c r="E109" s="5">
         <f t="shared" si="11"/>
         <v>9.1999999999999993</v>
       </c>
-      <c r="F108" s="5">
+      <c r="F109" s="5">
         <f t="shared" si="11"/>
         <v>7.666666666666667</v>
       </c>
-      <c r="G108" s="5">
+      <c r="G109" s="5">
         <f t="shared" si="11"/>
         <v>15.2</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E109" s="5"/>
-    </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E110" s="5"/>
     </row>
@@ -2216,268 +2264,267 @@
       <c r="E111" s="5"/>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
+      <c r="E112" s="5"/>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
         <v>61</v>
       </c>
-      <c r="B112">
+      <c r="B113">
         <v>561</v>
       </c>
-      <c r="C112" s="1">
+      <c r="C113" s="1">
         <v>561</v>
       </c>
-      <c r="E112" s="5">
-        <f t="shared" ref="E112:F124" si="12">B112/30</f>
+      <c r="E113" s="5">
+        <f t="shared" ref="E113:F125" si="12">B113/30</f>
         <v>18.7</v>
       </c>
-      <c r="F112" s="5">
+      <c r="F113" s="5">
         <f t="shared" si="12"/>
         <v>18.7</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
         <v>62</v>
       </c>
-      <c r="B113">
+      <c r="B114">
         <v>317</v>
       </c>
-      <c r="C113" s="1">
+      <c r="C114" s="1">
         <v>314</v>
       </c>
-      <c r="E113" s="5">
+      <c r="E114" s="5">
         <f t="shared" si="12"/>
         <v>10.566666666666666</v>
       </c>
-      <c r="F113" s="5">
+      <c r="F114" s="5">
         <f t="shared" si="12"/>
         <v>10.466666666666667</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
         <v>65</v>
       </c>
-      <c r="B114">
+      <c r="B115">
         <v>295</v>
       </c>
-      <c r="C114" s="1">
+      <c r="C115" s="1">
         <v>291</v>
       </c>
-      <c r="E114" s="5">
+      <c r="E115" s="5">
         <f t="shared" si="12"/>
         <v>9.8333333333333339</v>
       </c>
-      <c r="F114" s="5">
+      <c r="F115" s="5">
         <f t="shared" si="12"/>
         <v>9.6999999999999993</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E115" s="5"/>
-    </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
-        <v>67</v>
-      </c>
       <c r="E116" s="5"/>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
+        <v>67</v>
+      </c>
+      <c r="E117" s="5"/>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
         <v>61</v>
       </c>
-      <c r="B117">
+      <c r="B118">
         <v>553</v>
       </c>
-      <c r="C117" s="1">
+      <c r="C118" s="1">
         <v>554</v>
       </c>
-      <c r="E117" s="5">
+      <c r="E118" s="5">
         <f t="shared" si="12"/>
         <v>18.433333333333334</v>
       </c>
-      <c r="F117" s="5">
+      <c r="F118" s="5">
         <f t="shared" si="12"/>
         <v>18.466666666666665</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
         <v>62</v>
       </c>
-      <c r="B118">
+      <c r="B119">
         <v>311</v>
       </c>
-      <c r="C118" s="1">
+      <c r="C119" s="1">
         <v>317</v>
       </c>
-      <c r="E118" s="5">
+      <c r="E119" s="5">
         <f t="shared" si="12"/>
         <v>10.366666666666667</v>
       </c>
-      <c r="F118" s="5">
+      <c r="F119" s="5">
         <f t="shared" si="12"/>
         <v>10.566666666666666</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
         <v>65</v>
       </c>
-      <c r="B119">
+      <c r="B120">
         <v>292</v>
       </c>
-      <c r="C119" s="1">
+      <c r="C120" s="1">
         <v>288</v>
       </c>
-      <c r="E119" s="5">
+      <c r="E120" s="5">
         <f t="shared" si="12"/>
         <v>9.7333333333333325</v>
       </c>
-      <c r="F119" s="5">
+      <c r="F120" s="5">
         <f t="shared" si="12"/>
         <v>9.6</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E120" s="5"/>
-      <c r="F120" s="5"/>
-    </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
+      <c r="E121" s="5"/>
+      <c r="F121" s="5"/>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
         <v>68</v>
       </c>
-      <c r="B121">
+      <c r="B122">
         <v>381</v>
       </c>
-      <c r="E121" s="5">
+      <c r="E122" s="5">
         <f t="shared" si="12"/>
         <v>12.7</v>
       </c>
-      <c r="F121" s="5"/>
-    </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
+      <c r="F122" s="5"/>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
         <v>69</v>
       </c>
-      <c r="B122">
+      <c r="B123">
         <v>375</v>
       </c>
-      <c r="E122" s="5">
+      <c r="E123" s="5">
         <f t="shared" si="12"/>
         <v>12.5</v>
       </c>
-      <c r="F122" s="5"/>
-    </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E123" s="5"/>
       <c r="F123" s="5"/>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
+      <c r="E124" s="5"/>
+      <c r="F124" s="5"/>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
         <v>70</v>
       </c>
-      <c r="B124">
+      <c r="B125">
         <v>548</v>
       </c>
-      <c r="C124" s="1">
+      <c r="C125" s="1">
         <v>521</v>
       </c>
-      <c r="E124" s="5">
+      <c r="E125" s="5">
         <f t="shared" si="12"/>
         <v>18.266666666666666</v>
       </c>
-      <c r="F124" s="5">
+      <c r="F125" s="5">
         <f t="shared" si="12"/>
         <v>17.366666666666667</v>
       </c>
-      <c r="H124" s="2">
-        <f>B124/C124</f>
+      <c r="H125" s="2">
+        <f>B125/C125</f>
         <v>1.051823416506718</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B125">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B126">
         <v>309</v>
       </c>
-      <c r="C125" s="1">
+      <c r="C126" s="1">
         <v>305</v>
       </c>
-      <c r="E125" s="5">
-        <f t="shared" ref="E125:F136" si="13">B125/30</f>
+      <c r="E126" s="5">
+        <f t="shared" ref="E126:F141" si="13">B126/30</f>
         <v>10.3</v>
       </c>
-      <c r="F125" s="5">
+      <c r="F126" s="5">
         <f t="shared" si="13"/>
         <v>10.166666666666666</v>
       </c>
-      <c r="H125" s="2">
-        <f>B125/C125</f>
+      <c r="H126" s="2">
+        <f>B126/C126</f>
         <v>1.0131147540983607</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B126">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B127">
         <v>292</v>
       </c>
-      <c r="C126" s="1">
+      <c r="C127" s="1">
         <v>291</v>
       </c>
-      <c r="E126" s="5">
+      <c r="E127" s="5">
         <f t="shared" si="13"/>
         <v>9.7333333333333325</v>
       </c>
-      <c r="F126" s="5">
+      <c r="F127" s="5">
         <f t="shared" si="13"/>
         <v>9.6999999999999993</v>
       </c>
-      <c r="H126" s="2">
-        <f>B126/C126</f>
+      <c r="H127" s="2">
+        <f>B127/C127</f>
         <v>1.0034364261168385</v>
       </c>
-    </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E127" s="5"/>
-      <c r="F127" s="5"/>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E128" s="5"/>
       <c r="F128" s="5"/>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
+      <c r="E129" s="5"/>
+      <c r="F129" s="5"/>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
         <v>71</v>
       </c>
-      <c r="B129">
+      <c r="B130">
         <v>523</v>
       </c>
-      <c r="E129" s="5">
+      <c r="E130" s="5">
         <f t="shared" si="13"/>
         <v>17.433333333333334</v>
       </c>
-      <c r="F129" s="5"/>
-    </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B130">
+      <c r="F130" s="5"/>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B131">
         <v>288</v>
       </c>
-      <c r="E130" s="5">
+      <c r="E131" s="5">
         <f t="shared" si="13"/>
         <v>9.6</v>
       </c>
-      <c r="F130" s="5"/>
-    </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B131">
+      <c r="F131" s="5"/>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B132">
         <v>258</v>
       </c>
-      <c r="E131" s="5">
+      <c r="E132" s="5">
         <f t="shared" si="13"/>
         <v>8.6</v>
       </c>
-      <c r="F131" s="5"/>
-    </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E132" s="5"/>
       <c r="F132" s="5"/>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
@@ -2485,60 +2532,296 @@
       <c r="F133" s="5"/>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B134">
+      <c r="E134" s="5"/>
+      <c r="F134" s="5"/>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B135">
         <v>402</v>
       </c>
-      <c r="C134" s="1">
+      <c r="C135" s="1">
         <v>435</v>
       </c>
-      <c r="E134" s="5">
+      <c r="E135" s="5">
         <f t="shared" si="13"/>
         <v>13.4</v>
       </c>
-      <c r="F134" s="5">
+      <c r="F135" s="5">
         <f t="shared" si="13"/>
         <v>14.5</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B135">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B136">
         <v>225</v>
       </c>
-      <c r="C135" s="1">
+      <c r="C136" s="1">
         <v>268</v>
       </c>
-      <c r="E135" s="5">
+      <c r="E136" s="5">
         <f t="shared" si="13"/>
         <v>7.5</v>
       </c>
-      <c r="F135" s="5">
+      <c r="F136" s="5">
         <f t="shared" si="13"/>
         <v>8.9333333333333336</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B136">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B137">
         <v>206</v>
       </c>
-      <c r="C136" s="1">
+      <c r="C137" s="1">
         <v>226</v>
       </c>
-      <c r="E136" s="5">
+      <c r="E137" s="5">
         <f t="shared" si="13"/>
         <v>6.8666666666666663</v>
       </c>
-      <c r="F136" s="5">
+      <c r="F137" s="5">
         <f t="shared" si="13"/>
         <v>7.5333333333333332</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
+      <c r="E138" s="5"/>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
         <v>72</v>
+      </c>
+      <c r="B139">
+        <v>559</v>
+      </c>
+      <c r="E139" s="5">
+        <f t="shared" si="13"/>
+        <v>18.633333333333333</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B140">
+        <v>297</v>
+      </c>
+      <c r="E140" s="5">
+        <f t="shared" si="13"/>
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B141">
+        <v>269</v>
+      </c>
+      <c r="E141" s="5">
+        <f t="shared" si="13"/>
+        <v>8.9666666666666668</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E142" s="5"/>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E143" s="5"/>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>73</v>
+      </c>
+      <c r="B144">
+        <v>554</v>
+      </c>
+      <c r="E144" s="5">
+        <f t="shared" ref="E144:F158" si="14">B144/30</f>
+        <v>18.466666666666665</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B145">
+        <v>295</v>
+      </c>
+      <c r="E145" s="5">
+        <f t="shared" si="14"/>
+        <v>9.8333333333333339</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B146">
+        <v>256</v>
+      </c>
+      <c r="E146" s="5">
+        <f t="shared" si="14"/>
+        <v>8.5333333333333332</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E147" s="5"/>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>74</v>
+      </c>
+      <c r="B148">
+        <v>556</v>
+      </c>
+      <c r="C148" s="1">
+        <v>548</v>
+      </c>
+      <c r="E148" s="5">
+        <f t="shared" si="14"/>
+        <v>18.533333333333335</v>
+      </c>
+      <c r="F148" s="5">
+        <f t="shared" si="14"/>
+        <v>18.266666666666666</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B149">
+        <v>291</v>
+      </c>
+      <c r="E149" s="5">
+        <f t="shared" si="14"/>
+        <v>9.6999999999999993</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B150">
+        <v>262</v>
+      </c>
+      <c r="E150" s="5">
+        <f t="shared" si="14"/>
+        <v>8.7333333333333325</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E151" s="5"/>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>76</v>
+      </c>
+      <c r="B152">
+        <v>574</v>
+      </c>
+      <c r="E152" s="5">
+        <f t="shared" si="14"/>
+        <v>19.133333333333333</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B153">
+        <v>303</v>
+      </c>
+      <c r="E153" s="5">
+        <f t="shared" si="14"/>
+        <v>10.1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B154">
+        <v>265</v>
+      </c>
+      <c r="E154" s="5">
+        <f t="shared" si="14"/>
+        <v>8.8333333333333339</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E155" s="5"/>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>77</v>
+      </c>
+      <c r="B156">
+        <v>525</v>
+      </c>
+      <c r="E156" s="5">
+        <f t="shared" si="14"/>
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B157">
+        <v>285</v>
+      </c>
+      <c r="E157" s="5">
+        <f t="shared" si="14"/>
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B158">
+        <v>251</v>
+      </c>
+      <c r="E158" s="5">
+        <f t="shared" si="14"/>
+        <v>8.3666666666666671</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E159" s="5"/>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>78</v>
+      </c>
+      <c r="B160">
+        <v>611</v>
+      </c>
+      <c r="E160" s="5">
+        <f t="shared" ref="E160:E162" si="15">B160/30</f>
+        <v>20.366666666666667</v>
+      </c>
+    </row>
+    <row r="161" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B161">
+        <v>326</v>
+      </c>
+      <c r="E161" s="5">
+        <f t="shared" si="15"/>
+        <v>10.866666666666667</v>
+      </c>
+    </row>
+    <row r="162" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B162">
+        <v>330</v>
+      </c>
+      <c r="E162" s="5">
+        <f t="shared" si="15"/>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D6B7A93-A256-4135-9C93-B5E7687BF29D}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="3">
+        <v>18148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>26604</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Remove front to back rendering.
</commit_message>
<xml_diff>
--- a/P3DFps.xlsx
+++ b/P3DFps.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zak\Documents\GitProjects\Potato3d\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC4B2BA7-09E7-4E0A-95E8-C2B9B1370944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{844B30B5-D21C-46C5-B9B8-343CA1B22040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2904C00D-6B2E-49C9-A39A-1A4D989C3045}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="93">
   <si>
     <t>BSP</t>
   </si>
@@ -266,6 +266,45 @@
   </si>
   <si>
     <t>240X160</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cache </t>
+  </si>
+  <si>
+    <t>Misses</t>
+  </si>
+  <si>
+    <t>Peeks</t>
+  </si>
+  <si>
+    <t>Sorted Nodes</t>
+  </si>
+  <si>
+    <t>16x</t>
+  </si>
+  <si>
+    <t>8x</t>
+  </si>
+  <si>
+    <t>4x</t>
+  </si>
+  <si>
+    <t>Wide FOV</t>
+  </si>
+  <si>
+    <t>No tex cache</t>
+  </si>
+  <si>
+    <t>No Vx Cache</t>
+  </si>
+  <si>
+    <t>Obj3d IWRAM</t>
+  </si>
+  <si>
+    <t>Front to back</t>
+  </si>
+  <si>
+    <t>No early reject</t>
   </si>
 </sst>
 </file>
@@ -627,17 +666,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A9F04DC-EF96-45BA-9879-6DBCF76CA793}">
-  <dimension ref="A1:H162"/>
+  <dimension ref="A1:K197"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="F100" sqref="F100"/>
+    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
+      <selection activeCell="E177" sqref="E177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="1"/>
+    <col min="3" max="3" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.85546875" customWidth="1"/>
+    <col min="15" max="15" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -2769,11 +2810,11 @@
         <v>611</v>
       </c>
       <c r="E160" s="5">
-        <f t="shared" ref="E160:E162" si="15">B160/30</f>
+        <f t="shared" ref="E160:G173" si="15">B160/30</f>
         <v>20.366666666666667</v>
       </c>
     </row>
-    <row r="161" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B161">
         <v>326</v>
       </c>
@@ -2782,13 +2823,532 @@
         <v>10.866666666666667</v>
       </c>
     </row>
-    <row r="162" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B162">
         <v>330</v>
       </c>
       <c r="E162" s="5">
         <f t="shared" si="15"/>
         <v>11</v>
+      </c>
+    </row>
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E163" s="5"/>
+    </row>
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>84</v>
+      </c>
+      <c r="B164">
+        <v>366</v>
+      </c>
+      <c r="C164" s="1">
+        <v>263</v>
+      </c>
+      <c r="D164" s="4">
+        <v>273</v>
+      </c>
+      <c r="E164" s="5">
+        <f t="shared" si="15"/>
+        <v>12.2</v>
+      </c>
+      <c r="F164" s="5">
+        <f t="shared" si="15"/>
+        <v>8.7666666666666675</v>
+      </c>
+      <c r="G164" s="5">
+        <f t="shared" si="15"/>
+        <v>9.1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>85</v>
+      </c>
+      <c r="B165">
+        <v>355</v>
+      </c>
+      <c r="C165" s="1">
+        <v>255</v>
+      </c>
+      <c r="D165" s="4">
+        <v>263</v>
+      </c>
+      <c r="E165" s="5">
+        <f t="shared" si="15"/>
+        <v>11.833333333333334</v>
+      </c>
+      <c r="F165" s="5">
+        <f t="shared" ref="F165" si="16">C165/30</f>
+        <v>8.5</v>
+      </c>
+      <c r="G165" s="5">
+        <f t="shared" ref="G165" si="17">D165/30</f>
+        <v>8.7666666666666675</v>
+      </c>
+    </row>
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>86</v>
+      </c>
+      <c r="B166">
+        <v>359</v>
+      </c>
+      <c r="C166" s="1">
+        <v>259</v>
+      </c>
+      <c r="D166" s="4">
+        <v>268</v>
+      </c>
+      <c r="E166" s="5">
+        <f t="shared" si="15"/>
+        <v>11.966666666666667</v>
+      </c>
+      <c r="F166" s="5">
+        <f t="shared" si="15"/>
+        <v>8.6333333333333329</v>
+      </c>
+      <c r="G166" s="5">
+        <f t="shared" si="15"/>
+        <v>8.9333333333333336</v>
+      </c>
+    </row>
+    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>51</v>
+      </c>
+      <c r="B167">
+        <v>361</v>
+      </c>
+      <c r="C167" s="1">
+        <v>261</v>
+      </c>
+      <c r="D167" s="4"/>
+      <c r="E167" s="5">
+        <f t="shared" si="15"/>
+        <v>12.033333333333333</v>
+      </c>
+      <c r="F167" s="5">
+        <f t="shared" ref="F167" si="18">C167/30</f>
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="G167" s="5">
+        <f t="shared" ref="G167" si="19">D167/30</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D168" s="4"/>
+      <c r="E168" s="5"/>
+      <c r="F168" s="5"/>
+      <c r="G168" s="5"/>
+    </row>
+    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>87</v>
+      </c>
+      <c r="B169">
+        <v>295</v>
+      </c>
+      <c r="C169" s="1">
+        <v>238</v>
+      </c>
+      <c r="D169" s="4">
+        <v>247</v>
+      </c>
+      <c r="E169" s="5">
+        <f t="shared" si="15"/>
+        <v>9.8333333333333339</v>
+      </c>
+      <c r="F169" s="5">
+        <f t="shared" ref="F169" si="20">C169/30</f>
+        <v>7.9333333333333336</v>
+      </c>
+      <c r="G169" s="5">
+        <f t="shared" ref="G169" si="21">D169/30</f>
+        <v>8.2333333333333325</v>
+      </c>
+      <c r="I169" s="3">
+        <f>E169*254</f>
+        <v>2497.666666666667</v>
+      </c>
+      <c r="J169" s="3">
+        <f>F169*352</f>
+        <v>2792.5333333333333</v>
+      </c>
+      <c r="K169" s="3">
+        <f>G169*407</f>
+        <v>3350.9666666666662</v>
+      </c>
+    </row>
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>88</v>
+      </c>
+      <c r="B170">
+        <v>312</v>
+      </c>
+      <c r="C170" s="1">
+        <v>260</v>
+      </c>
+      <c r="D170" s="4">
+        <v>268</v>
+      </c>
+      <c r="E170" s="5">
+        <f t="shared" si="15"/>
+        <v>10.4</v>
+      </c>
+      <c r="F170" s="5">
+        <f t="shared" ref="F170:F173" si="22">C170/30</f>
+        <v>8.6666666666666661</v>
+      </c>
+      <c r="G170" s="5">
+        <f t="shared" ref="G170:G173" si="23">D170/30</f>
+        <v>8.9333333333333336</v>
+      </c>
+      <c r="I170" s="3">
+        <f t="shared" ref="I170:I177" si="24">E170*254</f>
+        <v>2641.6</v>
+      </c>
+      <c r="J170" s="3">
+        <f t="shared" ref="J170:J173" si="25">F170*352</f>
+        <v>3050.6666666666665</v>
+      </c>
+      <c r="K170" s="3">
+        <f t="shared" ref="K170:K173" si="26">G170*407</f>
+        <v>3635.8666666666668</v>
+      </c>
+    </row>
+    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>89</v>
+      </c>
+      <c r="B171">
+        <v>279</v>
+      </c>
+      <c r="C171" s="1">
+        <v>225</v>
+      </c>
+      <c r="D171" s="4">
+        <v>235</v>
+      </c>
+      <c r="E171" s="5">
+        <f t="shared" si="15"/>
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="F171" s="5">
+        <f t="shared" si="22"/>
+        <v>7.5</v>
+      </c>
+      <c r="G171" s="5">
+        <f t="shared" si="23"/>
+        <v>7.833333333333333</v>
+      </c>
+      <c r="I171" s="3">
+        <f t="shared" si="24"/>
+        <v>2362.2000000000003</v>
+      </c>
+      <c r="J171" s="3">
+        <f t="shared" si="25"/>
+        <v>2640</v>
+      </c>
+      <c r="K171" s="3">
+        <f t="shared" si="26"/>
+        <v>3188.1666666666665</v>
+      </c>
+    </row>
+    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>90</v>
+      </c>
+      <c r="B172">
+        <v>322</v>
+      </c>
+      <c r="C172" s="1">
+        <v>265</v>
+      </c>
+      <c r="D172" s="4">
+        <v>274</v>
+      </c>
+      <c r="E172" s="5">
+        <f t="shared" si="15"/>
+        <v>10.733333333333333</v>
+      </c>
+      <c r="F172" s="5">
+        <f t="shared" si="22"/>
+        <v>8.8333333333333339</v>
+      </c>
+      <c r="G172" s="5">
+        <f t="shared" si="23"/>
+        <v>9.1333333333333329</v>
+      </c>
+      <c r="I172" s="3">
+        <f t="shared" si="24"/>
+        <v>2726.2666666666664</v>
+      </c>
+      <c r="J172" s="3">
+        <f t="shared" si="25"/>
+        <v>3109.3333333333335</v>
+      </c>
+      <c r="K172" s="3">
+        <f t="shared" si="26"/>
+        <v>3717.2666666666664</v>
+      </c>
+    </row>
+    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>91</v>
+      </c>
+      <c r="B173">
+        <v>284</v>
+      </c>
+      <c r="C173" s="1">
+        <v>225</v>
+      </c>
+      <c r="D173" s="4">
+        <v>233</v>
+      </c>
+      <c r="E173" s="5">
+        <f t="shared" si="15"/>
+        <v>9.4666666666666668</v>
+      </c>
+      <c r="F173" s="5">
+        <f t="shared" si="22"/>
+        <v>7.5</v>
+      </c>
+      <c r="G173" s="5">
+        <f t="shared" si="23"/>
+        <v>7.7666666666666666</v>
+      </c>
+      <c r="I173" s="3">
+        <f t="shared" si="24"/>
+        <v>2404.5333333333333</v>
+      </c>
+      <c r="J173" s="3">
+        <f t="shared" si="25"/>
+        <v>2640</v>
+      </c>
+      <c r="K173" s="3">
+        <f t="shared" si="26"/>
+        <v>3161.0333333333333</v>
+      </c>
+    </row>
+    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D174" s="4"/>
+      <c r="E174" s="5"/>
+      <c r="F174" s="5"/>
+      <c r="G174" s="5"/>
+      <c r="I174" s="3"/>
+      <c r="J174" s="3"/>
+      <c r="K174" s="3"/>
+    </row>
+    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>92</v>
+      </c>
+      <c r="B175">
+        <v>310</v>
+      </c>
+      <c r="C175" s="1">
+        <v>238</v>
+      </c>
+      <c r="D175" s="4">
+        <v>229</v>
+      </c>
+      <c r="E175" s="5">
+        <f t="shared" ref="E175:E177" si="27">B175/30</f>
+        <v>10.333333333333334</v>
+      </c>
+      <c r="F175" s="5">
+        <f t="shared" ref="F175:F177" si="28">C175/30</f>
+        <v>7.9333333333333336</v>
+      </c>
+      <c r="G175" s="5">
+        <f t="shared" ref="G175:G177" si="29">D175/30</f>
+        <v>7.6333333333333337</v>
+      </c>
+      <c r="I175" s="3">
+        <f t="shared" si="24"/>
+        <v>2624.666666666667</v>
+      </c>
+      <c r="J175" s="3">
+        <f>F175*493</f>
+        <v>3911.1333333333337</v>
+      </c>
+      <c r="K175" s="3">
+        <f>G175*499</f>
+        <v>3809.0333333333338</v>
+      </c>
+    </row>
+    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B176">
+        <v>320</v>
+      </c>
+      <c r="C176" s="1">
+        <v>271</v>
+      </c>
+      <c r="D176" s="4">
+        <v>267</v>
+      </c>
+      <c r="E176" s="5">
+        <f t="shared" si="27"/>
+        <v>10.666666666666666</v>
+      </c>
+      <c r="F176" s="5">
+        <f t="shared" si="28"/>
+        <v>9.0333333333333332</v>
+      </c>
+      <c r="G176" s="5">
+        <f t="shared" si="29"/>
+        <v>8.9</v>
+      </c>
+      <c r="I176" s="3">
+        <f t="shared" si="24"/>
+        <v>2709.333333333333</v>
+      </c>
+      <c r="J176" s="3"/>
+      <c r="K176" s="3"/>
+    </row>
+    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B177">
+        <v>329</v>
+      </c>
+      <c r="C177" s="1">
+        <v>285</v>
+      </c>
+      <c r="D177" s="4">
+        <v>278</v>
+      </c>
+      <c r="E177" s="5">
+        <f t="shared" si="27"/>
+        <v>10.966666666666667</v>
+      </c>
+      <c r="F177" s="5">
+        <f t="shared" si="28"/>
+        <v>9.5</v>
+      </c>
+      <c r="G177" s="5">
+        <f t="shared" si="29"/>
+        <v>9.2666666666666675</v>
+      </c>
+      <c r="I177" s="3">
+        <f t="shared" si="24"/>
+        <v>2785.5333333333333</v>
+      </c>
+      <c r="K177" s="3"/>
+    </row>
+    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>82</v>
+      </c>
+      <c r="B179">
+        <v>357680</v>
+      </c>
+      <c r="C179" s="1">
+        <v>1156197</v>
+      </c>
+    </row>
+    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>81</v>
+      </c>
+      <c r="B180">
+        <v>17681</v>
+      </c>
+      <c r="C180" s="1">
+        <v>121609</v>
+      </c>
+    </row>
+    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B181" s="2">
+        <f>1-(B180/B179)</f>
+        <v>0.95056754641019903</v>
+      </c>
+      <c r="C181" s="2">
+        <f>1-(C180/C179)</f>
+        <v>0.89481982741695398</v>
+      </c>
+    </row>
+    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>83</v>
+      </c>
+      <c r="B183">
+        <v>191465</v>
+      </c>
+      <c r="C183" s="1">
+        <v>1191074</v>
+      </c>
+    </row>
+    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B184">
+        <v>9464</v>
+      </c>
+      <c r="C184" s="1">
+        <v>118945</v>
+      </c>
+    </row>
+    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B185" s="2">
+        <f>1-(B184/B183)</f>
+        <v>0.95057060037082497</v>
+      </c>
+      <c r="C185" s="2">
+        <f>1-(C184/C183)</f>
+        <v>0.90013634753172345</v>
+      </c>
+    </row>
+    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B191">
+        <v>1577090</v>
+      </c>
+      <c r="C191" s="1">
+        <v>1182119</v>
+      </c>
+      <c r="D191" s="2">
+        <f>C191/B191</f>
+        <v>0.74955709566353224</v>
+      </c>
+    </row>
+    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B192">
+        <v>1476188</v>
+      </c>
+      <c r="C192" s="1">
+        <v>1114233</v>
+      </c>
+      <c r="D192" s="2">
+        <f>C192/B192</f>
+        <v>0.75480426612328511</v>
+      </c>
+    </row>
+    <row r="194" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B194">
+        <v>4037321</v>
+      </c>
+      <c r="C194" s="1">
+        <v>1267009</v>
+      </c>
+      <c r="D194" s="2">
+        <f>C194/B194</f>
+        <v>0.31382419183413951</v>
+      </c>
+    </row>
+    <row r="197" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B197">
+        <v>4355914</v>
+      </c>
+      <c r="C197" s="1">
+        <v>2371658</v>
+      </c>
+      <c r="D197" s="2">
+        <f>C197/B197</f>
+        <v>0.54446850879057762</v>
       </c>
     </row>
   </sheetData>

</xml_diff>